<commit_message>
Fix locator for scenario 1
</commit_message>
<xml_diff>
--- a/Excel Files/Scenario 1/Expected Data/TC143/Expected Sales Order.xlsx
+++ b/Excel Files/Scenario 1/Expected Data/TC143/Expected Sales Order.xlsx
@@ -357,7 +357,7 @@
     <t>65-6222-3711</t>
   </si>
   <si>
-    <t>sCS201-2311001</t>
+    <t>sDS204-2311001</t>
   </si>
   <si>
     <t>Firm</t>
@@ -369,13 +369,13 @@
     <t>Weekly</t>
   </si>
   <si>
-    <t>06 Nov 2023 - 12 Nov 2023</t>
+    <t>27 Nov 2023 - 03 Dec 2023</t>
   </si>
   <si>
     <t>By Invoice Date</t>
   </si>
   <si>
-    <t>13 Nov ~ 19 Nov</t>
+    <t>04 Dec ~ 10 Dec</t>
   </si>
   <si>
     <t>FC Qty 1</t>
@@ -387,7 +387,7 @@
     <t>CNTW-SUP-POC-s1-001</t>
   </si>
   <si>
-    <t>pCS201-2311001</t>
+    <t>pDS204-2311001</t>
   </si>
   <si>
     <t>PK-CUS-POC</t>
@@ -9918,7 +9918,7 @@
         <v>60</v>
       </c>
       <c r="C18" s="29" t="n">
-        <v>45231.0</v>
+        <v>45250.0</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -10070,16 +10070,16 @@
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="2" t="n">
-        <v>45236.0</v>
+        <v>45251.0</v>
       </c>
       <c r="S23" s="2" t="n">
-        <v>45275.0</v>
+        <v>45293.0</v>
       </c>
       <c r="T23" s="2" t="n">
-        <v>45302.0</v>
+        <v>45331.0</v>
       </c>
       <c r="U23" s="2" t="n">
-        <v>45240.0</v>
+        <v>45265.0</v>
       </c>
     </row>
     <row r="24" spans="2:16">
@@ -10127,16 +10127,18 @@
         <v>1620.0</v>
       </c>
       <c r="Q24" s="42" t="n">
+        <v>1620.0</v>
+      </c>
+      <c r="R24" s="42" t="n">
         <v>0.0</v>
-      </c>
-      <c r="R24" s="42" t="n">
-        <v>1620.0</v>
       </c>
       <c r="S24" s="42" t="n">
         <v>1620.0</v>
       </c>
       <c r="T24" s="42"/>
-      <c r="U24" s="42"/>
+      <c r="U24" s="42" t="n">
+        <v>1620.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="25" t="s">
@@ -10183,16 +10185,18 @@
         <v>1620.0</v>
       </c>
       <c r="Q25" s="42" t="n">
+        <v>1620.0</v>
+      </c>
+      <c r="R25" s="42" t="n">
         <v>0.0</v>
-      </c>
-      <c r="R25" s="42" t="n">
-        <v>1620.0</v>
       </c>
       <c r="S25" s="42" t="n">
         <v>1620.0</v>
       </c>
       <c r="T25" s="42"/>
-      <c r="U25" s="42"/>
+      <c r="U25" s="42" t="n">
+        <v>1620.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="25" t="s">
@@ -10239,10 +10243,10 @@
         <v>800.0</v>
       </c>
       <c r="Q26" s="42" t="n">
-        <v>200.0</v>
+        <v>800.0</v>
       </c>
       <c r="R26" s="42" t="n">
-        <v>800.0</v>
+        <v>0.0</v>
       </c>
       <c r="S26" s="42" t="n">
         <v>600.0</v>
@@ -10251,7 +10255,7 @@
         <v>200.0</v>
       </c>
       <c r="U26" s="42" t="n">
-        <v>200.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="29">

</xml_diff>